<commit_message>
Upload revisions correcting spatial bounds at dataset level.
</commit_message>
<xml_diff>
--- a/MSB/LAGOS_NE_LIMNO_RAWDATA/ME_ANP_post_2006/ME_ANP_post_2006_attributes.xlsx
+++ b/MSB/LAGOS_NE_LIMNO_RAWDATA/ME_ANP_post_2006/ME_ANP_post_2006_attributes.xlsx
@@ -192,9 +192,6 @@
     <t>milligramsPerLiter</t>
   </si>
   <si>
-    <t>microequivlanetsPerLiter</t>
-  </si>
-  <si>
     <t>dimensionless</t>
   </si>
   <si>
@@ -331,6 +328,9 @@
   </si>
   <si>
     <t>Descriptor of reported value; E&lt; MRL number = Estimated value, actual value less than Method Reporting Level. &lt;MRLnumber = actual value less than Method Reporting Level.</t>
+  </si>
+  <si>
+    <t>microequivalentsPerLiter</t>
   </si>
 </sst>
 </file>
@@ -738,16 +738,16 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
         <v>53</v>
@@ -764,16 +764,16 @@
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" t="s">
         <v>53</v>
@@ -790,16 +790,16 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" t="s">
         <v>53</v>
@@ -816,16 +816,16 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
         <v>53</v>
@@ -845,16 +845,16 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
         <v>53</v>
@@ -868,13 +868,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -897,13 +897,13 @@
         <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8" t="s">
         <v>53</v>
@@ -923,16 +923,16 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -946,16 +946,16 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -969,16 +969,16 @@
         <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -992,13 +992,13 @@
         <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1012,16 +1012,16 @@
         <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1035,13 +1035,13 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1055,16 +1055,16 @@
         <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1078,13 +1078,13 @@
         <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1098,16 +1098,16 @@
         <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1118,16 +1118,16 @@
         <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1141,16 +1141,16 @@
         <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1164,13 +1164,13 @@
         <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1184,16 +1184,16 @@
         <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1207,13 +1207,13 @@
         <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1224,16 +1224,16 @@
         <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1244,16 +1244,16 @@
         <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1267,16 +1267,16 @@
         <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1290,13 +1290,13 @@
         <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1310,16 +1310,16 @@
         <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1330,16 +1330,16 @@
         <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1350,16 +1350,16 @@
         <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1373,16 +1373,16 @@
         <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1393,16 +1393,16 @@
         <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1413,16 +1413,16 @@
         <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1433,16 +1433,16 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1453,16 +1453,16 @@
         <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1473,16 +1473,16 @@
         <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1493,16 +1493,16 @@
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1513,16 +1513,16 @@
         <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1536,13 +1536,13 @@
         <v>56</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1556,16 +1556,16 @@
         <v>53</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1579,13 +1579,13 @@
         <v>56</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1599,16 +1599,16 @@
         <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1619,16 +1619,16 @@
         <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1642,16 +1642,16 @@
         <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1665,16 +1665,16 @@
         <v>53</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,16 +1688,16 @@
         <v>53</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>